<commit_message>
add colors TOPAZE and AMETHYSTE
</commit_message>
<xml_diff>
--- a/src/tournament/schedules/pool_A/schedule_aller.xlsx
+++ b/src/tournament/schedules/pool_A/schedule_aller.xlsx
@@ -32,6 +32,7 @@
       <b val="1"/>
     </font>
     <font>
+      <name val="Arial"/>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
@@ -39,7 +40,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -48,20 +49,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="004472C4"/>
-        <bgColor rgb="004472C4"/>
+        <fgColor rgb="00FFF8DC"/>
+        <bgColor rgb="00FFF8DC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BDD7EE"/>
-        <bgColor rgb="00BDD7EE"/>
+        <fgColor rgb="00996515"/>
+        <bgColor rgb="00996515"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E2EFDA"/>
-        <bgColor rgb="00E2EFDA"/>
+        <fgColor rgb="00FFE5B4"/>
+        <bgColor rgb="00FFE5B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFD700"/>
+        <bgColor rgb="00FFD700"/>
       </patternFill>
     </fill>
   </fills>
@@ -85,19 +92,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -478,44 +485,44 @@
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>round</t>
+          <t>Round</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>start_time</t>
+          <t>Début</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>end_time</t>
+          <t>Fin</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>team1</t>
+          <t>Équipe 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>team2</t>
+          <t>Équipe 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>duration</t>
+          <t>Durée</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>phase</t>
+          <t>Phase</t>
         </is>
       </c>
     </row>

</xml_diff>